<commit_message>
Sigmatron.xlsx; add Alex_sh as repaier
</commit_message>
<xml_diff>
--- a/Docs/ATE-2i10G for Sigmatron.xlsx
+++ b/Docs/ATE-2i10G for Sigmatron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63383D44-70E1-4753-9D93-75CC72001880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6BE7EB-82AF-4FD5-9A0F-3055143FD36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1185" windowWidth="20265" windowHeight="13845" xr2:uid="{F4EA2C0F-18A0-4F99-B7BC-942E21D7B492}"/>
+    <workbookView xWindow="7965" yWindow="885" windowWidth="20265" windowHeight="13845" xr2:uid="{F4EA2C0F-18A0-4F99-B7BC-942E21D7B492}"/>
   </bookViews>
   <sheets>
     <sheet name="Rack 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Product</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Barcode Scanner DS2208</t>
+  </si>
+  <si>
+    <t>ETX-2i-10G (RAD product, Golden Sample)</t>
+  </si>
+  <si>
+    <t>DF1003062694</t>
+  </si>
+  <si>
+    <t>Test Equipment (Power supply for JTAG station)</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -300,6 +309,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,8 +370,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C454C1F-FB2A-4B09-8E7A-4324D25A1D21}" name="Table1" displayName="Table1" ref="A4:F30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A4:F30" xr:uid="{4C454C1F-FB2A-4B09-8E7A-4324D25A1D21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C454C1F-FB2A-4B09-8E7A-4324D25A1D21}" name="Table1" displayName="Table1" ref="A4:F32" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A4:F32" xr:uid="{4C454C1F-FB2A-4B09-8E7A-4324D25A1D21}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{7D29B231-CF54-4C93-A1A0-1A3F8C21ED8C}" name="Product"/>
     <tableColumn id="3" xr3:uid="{3F953E00-6DF2-4BE0-BFA2-74ADFB18459A}" name="Price $USD" dataDxfId="4"/>
@@ -670,15 +683,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BA52B1-4968-4F2E-BE94-1D63F71DFA40}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
@@ -1123,22 +1136,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="2">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="13">
+        <v>540</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
       </c>
       <c r="D24" s="2">
         <f>C24*B24</f>
-        <v>2</v>
+        <v>540</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>7</v>
@@ -1146,38 +1159,38 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
       <c r="C25" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <f>C25*B25</f>
+        <v>2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2">
+        <f>C26*B26</f>
         <v>8</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" ref="D26:D29" si="4">C26*B26</f>
-        <v>6</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>38</v>
@@ -1188,17 +1201,17 @@
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2">
         <v>2</v>
       </c>
       <c r="D27" s="2">
-        <f>C27*B27</f>
-        <v>1</v>
+        <f t="shared" ref="D27:D31" si="4">C27*B27</f>
+        <v>6</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>38</v>
@@ -1207,19 +1220,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="2">
         <v>2</v>
-      </c>
-      <c r="C28" s="2">
-        <v>4</v>
       </c>
       <c r="D28" s="2">
         <f>C28*B28</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>38</v>
@@ -1230,39 +1243,81 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2">
+        <f>C29*B29</f>
+        <v>8</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="13">
+        <v>50</v>
+      </c>
+      <c r="C30" s="13">
+        <v>6</v>
+      </c>
+      <c r="D30" s="13">
+        <f>C30*B30</f>
+        <v>300</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B31" s="2">
         <v>450</v>
       </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="E31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="2">
-        <f>SUM(D5:D30)</f>
-        <v>4669</v>
-      </c>
-      <c r="F31" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="2">
+        <f>SUM(D5:D32)</f>
+        <v>5509</v>
+      </c>
+      <c r="F33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>